<commit_message>
Add updated calibreport template
</commit_message>
<xml_diff>
--- a/data/calibreport_template.xlsx
+++ b/data/calibreport_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\CCD\Data\spreadsheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zvanderbosch\data\CCD\Data\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC92C91F-8342-468A-8F09-7C8B5E5B02E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CC88C16-EC37-4A81-A609-580EA83DC93A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23580" yWindow="2820" windowWidth="18840" windowHeight="15420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4290" yWindow="1485" windowWidth="15585" windowHeight="20115" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="12" r:id="rId1"/>
@@ -89,9 +89,6 @@
     <t xml:space="preserve">NARRATIVE:  </t>
   </si>
   <si>
-    <t>SKY BRIGHTNESS DATA</t>
-  </si>
-  <si>
     <t xml:space="preserve">     Night Sky Quality Monitoring Report</t>
   </si>
   <si>
@@ -137,9 +134,6 @@
     <t>COLLECTION NOTES:</t>
   </si>
   <si>
-    <t>Zeropoint (mag)</t>
-  </si>
-  <si>
     <t>CALIBRATION FILES</t>
   </si>
   <si>
@@ -155,30 +149,12 @@
     <t>Average Platescale (arcsec/pix)</t>
   </si>
   <si>
-    <t>Plate Scale Adjustment Factor (mag)</t>
-  </si>
-  <si>
     <t>Extinction coefficient (mag/air-mass)</t>
   </si>
   <si>
     <t>Std Err Y Extinction Regression (mag)</t>
   </si>
   <si>
-    <t>Whole Sky         (mLux)     (mags)</t>
-  </si>
-  <si>
-    <t>Sky Above 20° Altitude (mags)</t>
-  </si>
-  <si>
-    <t>Brightest (mag/sq arc-sec)</t>
-  </si>
-  <si>
-    <t>Darkest (mag/sq arc-sec)</t>
-  </si>
-  <si>
-    <t>Zenith     (SKIES)    (mag/sq arcsec)</t>
-  </si>
-  <si>
     <t>Num Stars Extinction Regression</t>
   </si>
   <si>
@@ -188,10 +164,34 @@
     <t xml:space="preserve"> Folder name:</t>
   </si>
   <si>
-    <t>Sky Quality Index    Synthetic SQM</t>
-  </si>
-  <si>
-    <t>v.  07/01/2025</t>
+    <t>Zenith (mag/sq arcsec)</t>
+  </si>
+  <si>
+    <t>Plate Scale Adjustment  (mag)</t>
+  </si>
+  <si>
+    <t>Zeropoint Fixed    (mag)</t>
+  </si>
+  <si>
+    <t>Zeropoint Free     (mag)</t>
+  </si>
+  <si>
+    <t>EXTINCTION, POINTING, &amp; SKY BRIGHTNESS DATA</t>
+  </si>
+  <si>
+    <t>Average Pointing Error     (deg)</t>
+  </si>
+  <si>
+    <t>Brightest (mag/sq    arcsec)</t>
+  </si>
+  <si>
+    <t>Darkest (mag/sq    arcsec)</t>
+  </si>
+  <si>
+    <t>v.  07/08/2025</t>
+  </si>
+  <si>
+    <t>Synthetic SQM  (mag/sq arcsec)</t>
   </si>
 </sst>
 </file>
@@ -932,7 +932,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -962,9 +962,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -995,24 +992,12 @@
     <xf numFmtId="21" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="18" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="21" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="21" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1022,13 +1007,31 @@
     <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="18" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="19" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="20" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1058,16 +1061,16 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1130,12 +1133,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1220,10 +1217,7 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1306,156 +1300,6 @@
           <a:headEnd/>
           <a:tailEnd/>
         </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>119062</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>283368</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>488156</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>388143</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Picture 6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B762E41-AD2A-F2DA-DE9C-A743420D57EE}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5334000" y="5276056"/>
-          <a:ext cx="369094" cy="104775"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>120650</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>400049</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>489744</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>504824</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Picture 7">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{016D60F0-26C8-4E01-B496-460E53ECE06E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5934869" y="5392737"/>
-          <a:ext cx="369094" cy="104775"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>83344</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>298449</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>578827</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>403224</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Picture 8">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{942CF71D-A794-4B98-B60B-0ED253B7A33D}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8522494" y="5289549"/>
-          <a:ext cx="495483" cy="104775"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -1753,7 +1597,7 @@
   <dimension ref="A1:S36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection sqref="A1:N1"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1765,824 +1609,823 @@
     <col min="5" max="5" width="9.42578125" customWidth="1"/>
     <col min="6" max="6" width="9.85546875" customWidth="1"/>
     <col min="7" max="7" width="10.140625" customWidth="1"/>
-    <col min="8" max="8" width="9.28515625" customWidth="1"/>
-    <col min="9" max="9" width="9" customWidth="1"/>
+    <col min="8" max="9" width="9.5703125" customWidth="1"/>
     <col min="10" max="10" width="9.28515625" customWidth="1"/>
     <col min="11" max="14" width="10" customWidth="1"/>
     <col min="15" max="15" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="78" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
-      <c r="J1" s="78"/>
-      <c r="K1" s="78"/>
-      <c r="L1" s="78"/>
-      <c r="M1" s="78"/>
-      <c r="N1" s="78"/>
+      <c r="A1" s="77" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
+      <c r="L1" s="77"/>
+      <c r="M1" s="77"/>
+      <c r="N1" s="77"/>
     </row>
     <row r="2" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="96" t="s">
+      <c r="A2" s="95" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="95"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="95"/>
+      <c r="E2" s="95"/>
+      <c r="F2" s="95"/>
+      <c r="G2" s="95"/>
+      <c r="H2" s="95"/>
+      <c r="I2" s="95"/>
+      <c r="J2" s="95"/>
+      <c r="K2" s="95"/>
+      <c r="L2" s="95"/>
+      <c r="M2" s="95"/>
+      <c r="N2" s="95"/>
+    </row>
+    <row r="3" spans="1:14" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="96"/>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="96"/>
-      <c r="H2" s="96"/>
-      <c r="I2" s="96"/>
-      <c r="J2" s="96"/>
-      <c r="K2" s="96"/>
-      <c r="L2" s="96"/>
-      <c r="M2" s="96"/>
-      <c r="N2" s="96"/>
-    </row>
-    <row r="3" spans="1:14" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="D3" s="21"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="20"/>
       <c r="E3" s="5"/>
-      <c r="F3" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="G3" s="21"/>
+      <c r="F3" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="20"/>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
       <c r="M3" s="5"/>
-      <c r="N3" s="17" t="s">
-        <v>52</v>
+      <c r="N3" s="16" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="88" t="s">
+      <c r="A4" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="88"/>
-      <c r="C4" s="97"/>
-      <c r="D4" s="97"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="99" t="s">
+      <c r="B4" s="87"/>
+      <c r="C4" s="96"/>
+      <c r="D4" s="96"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="98" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="99"/>
-      <c r="H4" s="98"/>
-      <c r="I4" s="98"/>
-      <c r="J4" s="98"/>
-      <c r="K4" s="79"/>
-      <c r="L4" s="80"/>
-      <c r="M4" s="80"/>
-      <c r="N4" s="81"/>
+      <c r="G4" s="98"/>
+      <c r="H4" s="97"/>
+      <c r="I4" s="97"/>
+      <c r="J4" s="97"/>
+      <c r="K4" s="78"/>
+      <c r="L4" s="79"/>
+      <c r="M4" s="79"/>
+      <c r="N4" s="80"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="51" t="s">
+      <c r="A5" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="52"/>
-      <c r="C5" s="91"/>
-      <c r="D5" s="92"/>
+      <c r="B5" s="53"/>
+      <c r="C5" s="90"/>
+      <c r="D5" s="91"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="69" t="s">
+      <c r="F5" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="70"/>
-      <c r="H5" s="93"/>
-      <c r="I5" s="93"/>
-      <c r="J5" s="93"/>
-      <c r="K5" s="82"/>
-      <c r="L5" s="83"/>
-      <c r="M5" s="83"/>
-      <c r="N5" s="84"/>
+      <c r="G5" s="71"/>
+      <c r="H5" s="92"/>
+      <c r="I5" s="92"/>
+      <c r="J5" s="92"/>
+      <c r="K5" s="81"/>
+      <c r="L5" s="82"/>
+      <c r="M5" s="82"/>
+      <c r="N5" s="83"/>
     </row>
     <row r="6" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="51" t="s">
+      <c r="A6" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="52"/>
-      <c r="C6" s="91"/>
-      <c r="D6" s="92"/>
+      <c r="B6" s="53"/>
+      <c r="C6" s="90"/>
+      <c r="D6" s="91"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="69" t="s">
+      <c r="F6" s="70" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="70"/>
-      <c r="H6" s="93"/>
-      <c r="I6" s="93"/>
-      <c r="J6" s="93"/>
-      <c r="K6" s="82"/>
-      <c r="L6" s="83"/>
-      <c r="M6" s="83"/>
-      <c r="N6" s="84"/>
+      <c r="G6" s="71"/>
+      <c r="H6" s="92"/>
+      <c r="I6" s="92"/>
+      <c r="J6" s="92"/>
+      <c r="K6" s="81"/>
+      <c r="L6" s="82"/>
+      <c r="M6" s="82"/>
+      <c r="N6" s="83"/>
     </row>
     <row r="7" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="51" t="s">
+      <c r="A7" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="52"/>
-      <c r="C7" s="91"/>
-      <c r="D7" s="92"/>
+      <c r="B7" s="53"/>
+      <c r="C7" s="90"/>
+      <c r="D7" s="91"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="69" t="s">
+      <c r="F7" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="70"/>
-      <c r="H7" s="93"/>
-      <c r="I7" s="93"/>
-      <c r="J7" s="93"/>
-      <c r="K7" s="82"/>
-      <c r="L7" s="83"/>
-      <c r="M7" s="83"/>
-      <c r="N7" s="84"/>
+      <c r="G7" s="71"/>
+      <c r="H7" s="92"/>
+      <c r="I7" s="92"/>
+      <c r="J7" s="92"/>
+      <c r="K7" s="81"/>
+      <c r="L7" s="82"/>
+      <c r="M7" s="82"/>
+      <c r="N7" s="83"/>
     </row>
     <row r="8" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="51" t="s">
+      <c r="A8" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="52"/>
-      <c r="C8" s="91"/>
-      <c r="D8" s="92"/>
+      <c r="B8" s="53"/>
+      <c r="C8" s="90"/>
+      <c r="D8" s="91"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="69" t="s">
+      <c r="F8" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="70"/>
-      <c r="H8" s="93"/>
-      <c r="I8" s="93"/>
-      <c r="J8" s="93"/>
-      <c r="K8" s="82"/>
-      <c r="L8" s="83"/>
-      <c r="M8" s="83"/>
-      <c r="N8" s="84"/>
+      <c r="G8" s="71"/>
+      <c r="H8" s="92"/>
+      <c r="I8" s="92"/>
+      <c r="J8" s="92"/>
+      <c r="K8" s="81"/>
+      <c r="L8" s="82"/>
+      <c r="M8" s="82"/>
+      <c r="N8" s="83"/>
     </row>
     <row r="9" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="51" t="s">
+      <c r="A9" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="52"/>
-      <c r="C9" s="94"/>
-      <c r="D9" s="95"/>
+      <c r="B9" s="53"/>
+      <c r="C9" s="93"/>
+      <c r="D9" s="94"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="69" t="s">
+      <c r="F9" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="70"/>
-      <c r="H9" s="93"/>
-      <c r="I9" s="93"/>
-      <c r="J9" s="93"/>
-      <c r="K9" s="82"/>
-      <c r="L9" s="83"/>
-      <c r="M9" s="83"/>
-      <c r="N9" s="84"/>
+      <c r="G9" s="71"/>
+      <c r="H9" s="92"/>
+      <c r="I9" s="92"/>
+      <c r="J9" s="92"/>
+      <c r="K9" s="81"/>
+      <c r="L9" s="82"/>
+      <c r="M9" s="82"/>
+      <c r="N9" s="83"/>
     </row>
     <row r="10" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="51" t="s">
+      <c r="A10" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="52"/>
-      <c r="C10" s="89"/>
-      <c r="D10" s="90"/>
+      <c r="B10" s="53"/>
+      <c r="C10" s="88"/>
+      <c r="D10" s="89"/>
       <c r="E10" s="3"/>
-      <c r="F10" s="69" t="s">
+      <c r="F10" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="70"/>
-      <c r="H10" s="93"/>
-      <c r="I10" s="93"/>
-      <c r="J10" s="93"/>
-      <c r="K10" s="82"/>
-      <c r="L10" s="83"/>
-      <c r="M10" s="83"/>
-      <c r="N10" s="84"/>
+      <c r="G10" s="71"/>
+      <c r="H10" s="92"/>
+      <c r="I10" s="92"/>
+      <c r="J10" s="92"/>
+      <c r="K10" s="81"/>
+      <c r="L10" s="82"/>
+      <c r="M10" s="82"/>
+      <c r="N10" s="83"/>
     </row>
     <row r="11" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="51" t="s">
+      <c r="A11" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="52"/>
-      <c r="C11" s="91"/>
-      <c r="D11" s="92"/>
+      <c r="B11" s="53"/>
+      <c r="C11" s="90"/>
+      <c r="D11" s="91"/>
       <c r="E11" s="4"/>
-      <c r="F11" s="52" t="s">
+      <c r="F11" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="56"/>
+      <c r="G11" s="57"/>
       <c r="H11" s="6"/>
       <c r="I11" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J11" s="7"/>
-      <c r="K11" s="82"/>
-      <c r="L11" s="83"/>
-      <c r="M11" s="83"/>
-      <c r="N11" s="84"/>
+      <c r="K11" s="81"/>
+      <c r="L11" s="82"/>
+      <c r="M11" s="82"/>
+      <c r="N11" s="83"/>
     </row>
     <row r="12" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="56" t="s">
+      <c r="A12" s="57" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="57"/>
+      <c r="C12" s="58"/>
+      <c r="D12" s="58"/>
+      <c r="E12" s="58"/>
+      <c r="F12" s="58"/>
+      <c r="G12" s="58"/>
+      <c r="H12" s="58"/>
+      <c r="I12" s="58"/>
+      <c r="J12" s="58"/>
+      <c r="K12" s="81"/>
+      <c r="L12" s="82"/>
+      <c r="M12" s="82"/>
+      <c r="N12" s="83"/>
+    </row>
+    <row r="13" spans="1:14" ht="95.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="54" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="55"/>
+      <c r="C13" s="55"/>
+      <c r="D13" s="55"/>
+      <c r="E13" s="55"/>
+      <c r="F13" s="55"/>
+      <c r="G13" s="55"/>
+      <c r="H13" s="55"/>
+      <c r="I13" s="55"/>
+      <c r="J13" s="56"/>
+      <c r="K13" s="84"/>
+      <c r="L13" s="85"/>
+      <c r="M13" s="85"/>
+      <c r="N13" s="86"/>
+    </row>
+    <row r="14" spans="1:14" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="61" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="56"/>
-      <c r="C12" s="57"/>
-      <c r="D12" s="57"/>
-      <c r="E12" s="57"/>
-      <c r="F12" s="57"/>
-      <c r="G12" s="57"/>
-      <c r="H12" s="57"/>
-      <c r="I12" s="57"/>
-      <c r="J12" s="57"/>
-      <c r="K12" s="82"/>
-      <c r="L12" s="83"/>
-      <c r="M12" s="83"/>
-      <c r="N12" s="84"/>
-    </row>
-    <row r="13" spans="1:14" ht="95.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="53" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="54"/>
-      <c r="C13" s="54"/>
-      <c r="D13" s="54"/>
-      <c r="E13" s="54"/>
-      <c r="F13" s="54"/>
-      <c r="G13" s="54"/>
-      <c r="H13" s="54"/>
-      <c r="I13" s="54"/>
-      <c r="J13" s="55"/>
-      <c r="K13" s="85"/>
-      <c r="L13" s="86"/>
-      <c r="M13" s="86"/>
-      <c r="N13" s="87"/>
-    </row>
-    <row r="14" spans="1:14" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="60" t="s">
+      <c r="B14" s="61"/>
+      <c r="C14" s="61"/>
+      <c r="D14" s="61"/>
+      <c r="E14" s="61"/>
+      <c r="F14" s="61"/>
+      <c r="G14" s="61"/>
+      <c r="H14" s="61"/>
+      <c r="I14" s="61"/>
+      <c r="J14" s="61"/>
+      <c r="K14" s="61"/>
+      <c r="L14" s="61"/>
+      <c r="M14" s="61"/>
+      <c r="N14" s="61"/>
+    </row>
+    <row r="15" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="75" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="76"/>
+      <c r="C15" s="64"/>
+      <c r="D15" s="65"/>
+      <c r="E15" s="65"/>
+      <c r="F15" s="65"/>
+      <c r="G15" s="65"/>
+      <c r="H15" s="65"/>
+      <c r="I15" s="65"/>
+      <c r="J15" s="65"/>
+      <c r="K15" s="65"/>
+      <c r="L15" s="65"/>
+      <c r="M15" s="65"/>
+      <c r="N15" s="66"/>
+    </row>
+    <row r="16" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="62" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="63"/>
+      <c r="C16" s="67"/>
+      <c r="D16" s="68"/>
+      <c r="E16" s="68"/>
+      <c r="F16" s="68"/>
+      <c r="G16" s="68"/>
+      <c r="H16" s="68"/>
+      <c r="I16" s="68"/>
+      <c r="J16" s="68"/>
+      <c r="K16" s="68"/>
+      <c r="L16" s="68"/>
+      <c r="M16" s="68"/>
+      <c r="N16" s="69"/>
+    </row>
+    <row r="17" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="62" t="s">
         <v>35</v>
       </c>
-      <c r="B14" s="60"/>
-      <c r="C14" s="60"/>
-      <c r="D14" s="60"/>
-      <c r="E14" s="60"/>
-      <c r="F14" s="60"/>
-      <c r="G14" s="60"/>
-      <c r="H14" s="60"/>
-      <c r="I14" s="60"/>
-      <c r="J14" s="60"/>
-      <c r="K14" s="60"/>
-      <c r="L14" s="60"/>
-      <c r="M14" s="60"/>
-      <c r="N14" s="60"/>
-    </row>
-    <row r="15" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="76" t="s">
+      <c r="B17" s="63"/>
+      <c r="C17" s="67"/>
+      <c r="D17" s="68"/>
+      <c r="E17" s="68"/>
+      <c r="F17" s="68"/>
+      <c r="G17" s="68"/>
+      <c r="H17" s="68"/>
+      <c r="I17" s="68"/>
+      <c r="J17" s="68"/>
+      <c r="K17" s="68"/>
+      <c r="L17" s="68"/>
+      <c r="M17" s="68"/>
+      <c r="N17" s="69"/>
+    </row>
+    <row r="18" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="77"/>
-      <c r="C15" s="63"/>
-      <c r="D15" s="64"/>
-      <c r="E15" s="64"/>
-      <c r="F15" s="64"/>
-      <c r="G15" s="64"/>
-      <c r="H15" s="64"/>
-      <c r="I15" s="64"/>
-      <c r="J15" s="64"/>
-      <c r="K15" s="64"/>
-      <c r="L15" s="64"/>
-      <c r="M15" s="64"/>
-      <c r="N15" s="65"/>
-    </row>
-    <row r="16" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="61" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="62"/>
-      <c r="C16" s="66"/>
-      <c r="D16" s="67"/>
-      <c r="E16" s="67"/>
-      <c r="F16" s="67"/>
-      <c r="G16" s="67"/>
-      <c r="H16" s="67"/>
-      <c r="I16" s="67"/>
-      <c r="J16" s="67"/>
-      <c r="K16" s="67"/>
-      <c r="L16" s="67"/>
-      <c r="M16" s="67"/>
-      <c r="N16" s="68"/>
-    </row>
-    <row r="17" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="61" t="s">
-        <v>37</v>
-      </c>
-      <c r="B17" s="62"/>
-      <c r="C17" s="66"/>
-      <c r="D17" s="67"/>
-      <c r="E17" s="67"/>
-      <c r="F17" s="67"/>
-      <c r="G17" s="67"/>
-      <c r="H17" s="67"/>
-      <c r="I17" s="67"/>
-      <c r="J17" s="67"/>
-      <c r="K17" s="67"/>
-      <c r="L17" s="67"/>
-      <c r="M17" s="67"/>
-      <c r="N17" s="68"/>
-    </row>
-    <row r="18" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="54" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="55"/>
-      <c r="C18" s="73"/>
-      <c r="D18" s="74"/>
-      <c r="E18" s="74"/>
-      <c r="F18" s="74"/>
-      <c r="G18" s="74"/>
-      <c r="H18" s="74"/>
-      <c r="I18" s="74"/>
-      <c r="J18" s="74"/>
-      <c r="K18" s="74"/>
-      <c r="L18" s="74"/>
-      <c r="M18" s="74"/>
-      <c r="N18" s="75"/>
+      <c r="B18" s="56"/>
+      <c r="C18" s="72"/>
+      <c r="D18" s="73"/>
+      <c r="E18" s="73"/>
+      <c r="F18" s="73"/>
+      <c r="G18" s="73"/>
+      <c r="H18" s="73"/>
+      <c r="I18" s="73"/>
+      <c r="J18" s="73"/>
+      <c r="K18" s="73"/>
+      <c r="L18" s="73"/>
+      <c r="M18" s="73"/>
+      <c r="N18" s="74"/>
     </row>
     <row r="19" spans="1:19" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="58" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" s="58"/>
-      <c r="C19" s="58"/>
-      <c r="D19" s="58"/>
-      <c r="E19" s="58"/>
-      <c r="F19" s="58"/>
-      <c r="G19" s="58"/>
-      <c r="H19" s="58"/>
-      <c r="I19" s="58"/>
-      <c r="J19" s="58"/>
-      <c r="K19" s="58"/>
-      <c r="L19" s="58"/>
-      <c r="M19" s="58"/>
-      <c r="N19" s="59"/>
+      <c r="A19" s="59" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="59"/>
+      <c r="C19" s="59"/>
+      <c r="D19" s="59"/>
+      <c r="E19" s="59"/>
+      <c r="F19" s="59"/>
+      <c r="G19" s="59"/>
+      <c r="H19" s="59"/>
+      <c r="I19" s="59"/>
+      <c r="J19" s="59"/>
+      <c r="K19" s="59"/>
+      <c r="L19" s="59"/>
+      <c r="M19" s="59"/>
+      <c r="N19" s="60"/>
     </row>
     <row r="20" spans="1:19" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="8" t="s">
-        <v>31</v>
-      </c>
       <c r="C20" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D20" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="F20" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="G20" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="H20" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="I20" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="J20" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="G20" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="H20" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="I20" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="J20" s="12" t="s">
+      <c r="K20" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="K20" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="L20" s="14" t="s">
-        <v>45</v>
+      <c r="L20" s="13" t="s">
+        <v>49</v>
       </c>
       <c r="M20" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="N20" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="O20" s="32"/>
-      <c r="P20" s="19"/>
-      <c r="Q20" s="19"/>
-      <c r="R20" s="19"/>
-      <c r="S20" s="19"/>
+        <v>50</v>
+      </c>
+      <c r="N20" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="O20" s="27"/>
+      <c r="P20" s="18"/>
+      <c r="Q20" s="18"/>
+      <c r="R20" s="18"/>
+      <c r="S20" s="18"/>
     </row>
     <row r="21" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="43" t="s">
+      <c r="A21" s="44" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="24"/>
+      <c r="C21" s="46"/>
+      <c r="D21" s="48"/>
+      <c r="E21" s="33"/>
+      <c r="F21" s="33"/>
+      <c r="G21" s="50"/>
+      <c r="H21" s="33"/>
+      <c r="I21" s="33"/>
+      <c r="J21" s="36"/>
+      <c r="K21" s="39"/>
+      <c r="L21" s="39"/>
+      <c r="M21" s="39"/>
+      <c r="N21" s="30"/>
+      <c r="O21" s="29"/>
+      <c r="P21" s="18"/>
+      <c r="Q21" s="18"/>
+      <c r="R21" s="18"/>
+      <c r="S21" s="18"/>
+    </row>
+    <row r="22" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="45"/>
+      <c r="B22" s="25"/>
+      <c r="C22" s="47"/>
+      <c r="D22" s="49"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="34"/>
+      <c r="G22" s="51"/>
+      <c r="H22" s="34"/>
+      <c r="I22" s="34"/>
+      <c r="J22" s="37"/>
+      <c r="K22" s="40"/>
+      <c r="L22" s="40"/>
+      <c r="M22" s="40"/>
+      <c r="N22" s="31"/>
+      <c r="O22" s="29"/>
+      <c r="P22" s="18"/>
+      <c r="Q22" s="18"/>
+      <c r="R22" s="18"/>
+      <c r="S22" s="18"/>
+    </row>
+    <row r="23" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="25"/>
-      <c r="C21" s="45"/>
-      <c r="D21" s="47"/>
-      <c r="E21" s="49"/>
-      <c r="F21" s="71"/>
-      <c r="G21" s="49"/>
-      <c r="H21" s="49"/>
-      <c r="I21" s="26"/>
-      <c r="J21" s="27"/>
-      <c r="K21" s="38"/>
-      <c r="L21" s="38"/>
-      <c r="M21" s="38"/>
-      <c r="N21" s="37"/>
-      <c r="O21" s="34"/>
-      <c r="P21" s="19"/>
-      <c r="Q21" s="19"/>
-      <c r="R21" s="19"/>
-      <c r="S21" s="19"/>
-    </row>
-    <row r="22" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="44"/>
-      <c r="B22" s="28"/>
-      <c r="C22" s="46"/>
-      <c r="D22" s="48"/>
-      <c r="E22" s="50"/>
-      <c r="F22" s="72"/>
-      <c r="G22" s="50"/>
-      <c r="H22" s="50"/>
-      <c r="I22" s="29"/>
-      <c r="J22" s="29"/>
-      <c r="K22" s="39"/>
-      <c r="L22" s="39"/>
-      <c r="M22" s="39"/>
-      <c r="N22" s="35"/>
-      <c r="O22" s="34"/>
-      <c r="P22" s="19"/>
-      <c r="Q22" s="19"/>
-      <c r="R22" s="19"/>
-      <c r="S22" s="19"/>
-    </row>
-    <row r="23" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" s="25"/>
-      <c r="C23" s="45"/>
-      <c r="D23" s="47"/>
-      <c r="E23" s="49"/>
-      <c r="F23" s="71"/>
-      <c r="G23" s="49"/>
-      <c r="H23" s="49"/>
-      <c r="I23" s="26" t="str">
+      <c r="B23" s="24"/>
+      <c r="C23" s="46"/>
+      <c r="D23" s="48"/>
+      <c r="E23" s="33"/>
+      <c r="F23" s="33"/>
+      <c r="G23" s="50"/>
+      <c r="H23" s="33"/>
+      <c r="I23" s="33" t="str">
         <f>IF(I24="","",(108468000*POWER(10,-0.4*I24))/0.171918)</f>
         <v/>
       </c>
-      <c r="J23" s="27" t="str">
+      <c r="J23" s="36" t="str">
         <f>IF(J24="","",0.00254*(POWER(10,(-0.4*J24))))</f>
         <v/>
       </c>
-      <c r="K23" s="38"/>
-      <c r="L23" s="38"/>
-      <c r="M23" s="38"/>
-      <c r="N23" s="37"/>
-      <c r="O23" s="34"/>
-      <c r="P23" s="19"/>
-      <c r="Q23" s="19"/>
-      <c r="R23" s="19"/>
-      <c r="S23" s="19"/>
+      <c r="K23" s="39"/>
+      <c r="L23" s="39"/>
+      <c r="M23" s="39"/>
+      <c r="N23" s="30"/>
+      <c r="O23" s="29"/>
+      <c r="P23" s="18"/>
+      <c r="Q23" s="18"/>
+      <c r="R23" s="18"/>
+      <c r="S23" s="18"/>
     </row>
     <row r="24" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="44"/>
-      <c r="B24" s="28"/>
-      <c r="C24" s="46"/>
-      <c r="D24" s="48"/>
-      <c r="E24" s="50"/>
-      <c r="F24" s="72"/>
-      <c r="G24" s="50"/>
-      <c r="H24" s="50"/>
-      <c r="I24" s="29"/>
-      <c r="J24" s="29"/>
-      <c r="K24" s="39"/>
-      <c r="L24" s="39"/>
-      <c r="M24" s="39"/>
-      <c r="N24" s="35"/>
-      <c r="O24" s="34"/>
-      <c r="P24" s="19"/>
-      <c r="Q24" s="19"/>
-      <c r="R24" s="19"/>
-      <c r="S24" s="19"/>
+      <c r="A24" s="45"/>
+      <c r="B24" s="25"/>
+      <c r="C24" s="47"/>
+      <c r="D24" s="49"/>
+      <c r="E24" s="34"/>
+      <c r="F24" s="34"/>
+      <c r="G24" s="51"/>
+      <c r="H24" s="34"/>
+      <c r="I24" s="34"/>
+      <c r="J24" s="37"/>
+      <c r="K24" s="40"/>
+      <c r="L24" s="40"/>
+      <c r="M24" s="40"/>
+      <c r="N24" s="31"/>
+      <c r="O24" s="29"/>
+      <c r="P24" s="18"/>
+      <c r="Q24" s="18"/>
+      <c r="R24" s="18"/>
+      <c r="S24" s="18"/>
     </row>
     <row r="25" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="43" t="s">
-        <v>24</v>
-      </c>
-      <c r="B25" s="25"/>
-      <c r="C25" s="45"/>
-      <c r="D25" s="47"/>
-      <c r="E25" s="49"/>
-      <c r="F25" s="71"/>
-      <c r="G25" s="49"/>
-      <c r="H25" s="49"/>
-      <c r="I25" s="26" t="str">
+      <c r="A25" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="24"/>
+      <c r="C25" s="46"/>
+      <c r="D25" s="48"/>
+      <c r="E25" s="33"/>
+      <c r="F25" s="33"/>
+      <c r="G25" s="50"/>
+      <c r="H25" s="33"/>
+      <c r="I25" s="33" t="str">
         <f>IF(I26="","",(108468000*POWER(10,-0.4*I26))/0.171918)</f>
         <v/>
       </c>
-      <c r="J25" s="27" t="str">
+      <c r="J25" s="36" t="str">
         <f>IF(J26="","",0.00254*(POWER(10,(-0.4*J26))))</f>
         <v/>
       </c>
-      <c r="K25" s="38"/>
-      <c r="L25" s="38"/>
-      <c r="M25" s="38"/>
-      <c r="N25" s="37"/>
-      <c r="O25" s="34"/>
-      <c r="P25" s="19"/>
-      <c r="Q25" s="19"/>
-      <c r="R25" s="19"/>
-      <c r="S25" s="19"/>
+      <c r="K25" s="39"/>
+      <c r="L25" s="39"/>
+      <c r="M25" s="39"/>
+      <c r="N25" s="30"/>
+      <c r="O25" s="29"/>
+      <c r="P25" s="18"/>
+      <c r="Q25" s="18"/>
+      <c r="R25" s="18"/>
+      <c r="S25" s="18"/>
     </row>
     <row r="26" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="44"/>
-      <c r="B26" s="28"/>
-      <c r="C26" s="46"/>
-      <c r="D26" s="48"/>
-      <c r="E26" s="50"/>
-      <c r="F26" s="72"/>
-      <c r="G26" s="50"/>
-      <c r="H26" s="50"/>
-      <c r="I26" s="29"/>
-      <c r="J26" s="29"/>
-      <c r="K26" s="39"/>
-      <c r="L26" s="39"/>
-      <c r="M26" s="39"/>
-      <c r="N26" s="35"/>
-      <c r="O26" s="34"/>
-      <c r="P26" s="19"/>
-      <c r="Q26" s="19"/>
-      <c r="R26" s="19"/>
-      <c r="S26" s="19"/>
+      <c r="A26" s="45"/>
+      <c r="B26" s="25"/>
+      <c r="C26" s="47"/>
+      <c r="D26" s="49"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="34"/>
+      <c r="G26" s="51"/>
+      <c r="H26" s="34"/>
+      <c r="I26" s="34"/>
+      <c r="J26" s="37"/>
+      <c r="K26" s="40"/>
+      <c r="L26" s="40"/>
+      <c r="M26" s="40"/>
+      <c r="N26" s="31"/>
+      <c r="O26" s="29"/>
+      <c r="P26" s="18"/>
+      <c r="Q26" s="18"/>
+      <c r="R26" s="18"/>
+      <c r="S26" s="18"/>
     </row>
     <row r="27" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="43" t="s">
-        <v>25</v>
-      </c>
-      <c r="B27" s="25"/>
-      <c r="C27" s="45"/>
-      <c r="D27" s="47"/>
-      <c r="E27" s="49"/>
-      <c r="F27" s="71"/>
-      <c r="G27" s="49"/>
-      <c r="H27" s="49"/>
-      <c r="I27" s="26" t="str">
+      <c r="A27" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" s="24"/>
+      <c r="C27" s="46"/>
+      <c r="D27" s="48"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="33"/>
+      <c r="G27" s="50"/>
+      <c r="H27" s="33"/>
+      <c r="I27" s="33" t="str">
         <f>IF(I28="","",(108468000*POWER(10,-0.4*I28))/0.171918)</f>
         <v/>
       </c>
-      <c r="J27" s="27" t="str">
+      <c r="J27" s="36" t="str">
         <f>IF(J28="","",0.00254*(POWER(10,(-0.4*J28))))</f>
         <v/>
       </c>
-      <c r="K27" s="38"/>
-      <c r="L27" s="38"/>
-      <c r="M27" s="38"/>
-      <c r="N27" s="37"/>
-      <c r="O27" s="34"/>
-      <c r="P27" s="19"/>
-      <c r="Q27" s="19"/>
-      <c r="R27" s="19"/>
-      <c r="S27" s="19"/>
+      <c r="K27" s="39"/>
+      <c r="L27" s="39"/>
+      <c r="M27" s="39"/>
+      <c r="N27" s="30"/>
+      <c r="O27" s="29"/>
+      <c r="P27" s="18"/>
+      <c r="Q27" s="18"/>
+      <c r="R27" s="18"/>
+      <c r="S27" s="18"/>
     </row>
     <row r="28" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="44"/>
-      <c r="B28" s="28"/>
-      <c r="C28" s="46"/>
-      <c r="D28" s="48"/>
-      <c r="E28" s="50"/>
-      <c r="F28" s="72"/>
-      <c r="G28" s="50"/>
-      <c r="H28" s="50"/>
-      <c r="I28" s="29"/>
-      <c r="J28" s="29"/>
-      <c r="K28" s="39"/>
-      <c r="L28" s="39"/>
-      <c r="M28" s="39"/>
-      <c r="N28" s="35"/>
-      <c r="O28" s="34"/>
-      <c r="P28" s="19"/>
-      <c r="Q28" s="19"/>
-      <c r="R28" s="19"/>
-      <c r="S28" s="19"/>
+      <c r="A28" s="45"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="47"/>
+      <c r="D28" s="49"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="34"/>
+      <c r="G28" s="51"/>
+      <c r="H28" s="34"/>
+      <c r="I28" s="34"/>
+      <c r="J28" s="37"/>
+      <c r="K28" s="40"/>
+      <c r="L28" s="40"/>
+      <c r="M28" s="40"/>
+      <c r="N28" s="31"/>
+      <c r="O28" s="29"/>
+      <c r="P28" s="18"/>
+      <c r="Q28" s="18"/>
+      <c r="R28" s="18"/>
+      <c r="S28" s="18"/>
     </row>
     <row r="29" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="43" t="s">
-        <v>26</v>
-      </c>
-      <c r="B29" s="25"/>
-      <c r="C29" s="45"/>
-      <c r="D29" s="47"/>
-      <c r="E29" s="49"/>
-      <c r="F29" s="71"/>
-      <c r="G29" s="49"/>
-      <c r="H29" s="49"/>
-      <c r="I29" s="26" t="str">
+      <c r="A29" s="44" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29" s="24"/>
+      <c r="C29" s="46"/>
+      <c r="D29" s="48"/>
+      <c r="E29" s="33"/>
+      <c r="F29" s="33"/>
+      <c r="G29" s="50"/>
+      <c r="H29" s="33"/>
+      <c r="I29" s="33" t="str">
         <f>IF(I30="","",(108468000*POWER(10,-0.4*I30))/0.171918)</f>
         <v/>
       </c>
-      <c r="J29" s="27" t="str">
+      <c r="J29" s="36" t="str">
         <f>IF(J30="","",0.00254*(POWER(10,(-0.4*J30))))</f>
         <v/>
       </c>
-      <c r="K29" s="38"/>
-      <c r="L29" s="38"/>
-      <c r="M29" s="38"/>
-      <c r="N29" s="37"/>
-      <c r="O29" s="34"/>
-      <c r="P29" s="19"/>
-      <c r="Q29" s="19"/>
-      <c r="R29" s="19"/>
-      <c r="S29" s="19"/>
+      <c r="K29" s="39"/>
+      <c r="L29" s="39"/>
+      <c r="M29" s="39"/>
+      <c r="N29" s="30"/>
+      <c r="O29" s="29"/>
+      <c r="P29" s="18"/>
+      <c r="Q29" s="18"/>
+      <c r="R29" s="18"/>
+      <c r="S29" s="18"/>
     </row>
     <row r="30" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="44"/>
-      <c r="B30" s="28"/>
-      <c r="C30" s="46"/>
-      <c r="D30" s="48"/>
-      <c r="E30" s="50"/>
-      <c r="F30" s="72"/>
-      <c r="G30" s="50"/>
-      <c r="H30" s="50"/>
-      <c r="I30" s="29"/>
-      <c r="J30" s="29"/>
-      <c r="K30" s="39"/>
-      <c r="L30" s="39"/>
-      <c r="M30" s="39"/>
-      <c r="N30" s="35"/>
-      <c r="O30" s="34"/>
-      <c r="P30" s="19"/>
-      <c r="Q30" s="19"/>
-      <c r="R30" s="19"/>
-      <c r="S30" s="19"/>
+      <c r="A30" s="45"/>
+      <c r="B30" s="25"/>
+      <c r="C30" s="47"/>
+      <c r="D30" s="49"/>
+      <c r="E30" s="34"/>
+      <c r="F30" s="34"/>
+      <c r="G30" s="51"/>
+      <c r="H30" s="34"/>
+      <c r="I30" s="34"/>
+      <c r="J30" s="37"/>
+      <c r="K30" s="40"/>
+      <c r="L30" s="40"/>
+      <c r="M30" s="40"/>
+      <c r="N30" s="31"/>
+      <c r="O30" s="29"/>
+      <c r="P30" s="18"/>
+      <c r="Q30" s="18"/>
+      <c r="R30" s="18"/>
+      <c r="S30" s="18"/>
     </row>
     <row r="31" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="43" t="s">
-        <v>27</v>
-      </c>
-      <c r="B31" s="25"/>
-      <c r="C31" s="45"/>
-      <c r="D31" s="47"/>
-      <c r="E31" s="49"/>
-      <c r="F31" s="71"/>
-      <c r="G31" s="49"/>
-      <c r="H31" s="49"/>
-      <c r="I31" s="26" t="str">
+      <c r="A31" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31" s="24"/>
+      <c r="C31" s="46"/>
+      <c r="D31" s="48"/>
+      <c r="E31" s="33"/>
+      <c r="F31" s="33"/>
+      <c r="G31" s="50"/>
+      <c r="H31" s="33"/>
+      <c r="I31" s="33" t="str">
         <f>IF(I32="","",(108468000*POWER(10,-0.4*I32))/0.171918)</f>
         <v/>
       </c>
-      <c r="J31" s="27" t="str">
+      <c r="J31" s="36" t="str">
         <f>IF(J32="","",0.00254*(POWER(10,(-0.4*J32))))</f>
         <v/>
       </c>
-      <c r="K31" s="38"/>
-      <c r="L31" s="38"/>
-      <c r="M31" s="38"/>
-      <c r="N31" s="37"/>
-      <c r="O31" s="34"/>
-      <c r="P31" s="19"/>
-      <c r="Q31" s="19"/>
-      <c r="R31" s="19"/>
-      <c r="S31" s="19"/>
+      <c r="K31" s="39"/>
+      <c r="L31" s="39"/>
+      <c r="M31" s="39"/>
+      <c r="N31" s="30"/>
+      <c r="O31" s="29"/>
+      <c r="P31" s="18"/>
+      <c r="Q31" s="18"/>
+      <c r="R31" s="18"/>
+      <c r="S31" s="18"/>
     </row>
     <row r="32" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="44"/>
-      <c r="B32" s="28"/>
-      <c r="C32" s="46"/>
-      <c r="D32" s="48"/>
-      <c r="E32" s="50"/>
-      <c r="F32" s="72"/>
-      <c r="G32" s="50"/>
-      <c r="H32" s="50"/>
-      <c r="I32" s="29"/>
-      <c r="J32" s="29"/>
-      <c r="K32" s="39"/>
-      <c r="L32" s="39"/>
-      <c r="M32" s="39"/>
-      <c r="N32" s="35"/>
-      <c r="O32" s="34"/>
-      <c r="P32" s="19"/>
-      <c r="Q32" s="19"/>
-      <c r="R32" s="19"/>
-      <c r="S32" s="19"/>
+      <c r="A32" s="45"/>
+      <c r="B32" s="25"/>
+      <c r="C32" s="47"/>
+      <c r="D32" s="49"/>
+      <c r="E32" s="34"/>
+      <c r="F32" s="34"/>
+      <c r="G32" s="51"/>
+      <c r="H32" s="34"/>
+      <c r="I32" s="34"/>
+      <c r="J32" s="37"/>
+      <c r="K32" s="40"/>
+      <c r="L32" s="40"/>
+      <c r="M32" s="40"/>
+      <c r="N32" s="31"/>
+      <c r="O32" s="29"/>
+      <c r="P32" s="18"/>
+      <c r="Q32" s="18"/>
+      <c r="R32" s="18"/>
+      <c r="S32" s="18"/>
     </row>
     <row r="33" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="41" t="s">
-        <v>28</v>
-      </c>
-      <c r="B33" s="25"/>
-      <c r="C33" s="45"/>
-      <c r="D33" s="47"/>
-      <c r="E33" s="49"/>
-      <c r="F33" s="71"/>
-      <c r="G33" s="49"/>
-      <c r="H33" s="49"/>
-      <c r="I33" s="26" t="str">
+      <c r="A33" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="B33" s="24"/>
+      <c r="C33" s="46"/>
+      <c r="D33" s="48"/>
+      <c r="E33" s="33"/>
+      <c r="F33" s="33"/>
+      <c r="G33" s="50"/>
+      <c r="H33" s="33"/>
+      <c r="I33" s="33" t="str">
         <f>IF(I34="","",(108468000*POWER(10,-0.4*I34))/0.171918)</f>
         <v/>
       </c>
-      <c r="J33" s="27" t="str">
+      <c r="J33" s="36" t="str">
         <f>IF(J34="","",0.00254*(POWER(10,(-0.4*J34))))</f>
         <v/>
       </c>
-      <c r="K33" s="38"/>
-      <c r="L33" s="38"/>
-      <c r="M33" s="38"/>
-      <c r="N33" s="37"/>
-      <c r="O33" s="34"/>
-      <c r="P33" s="19"/>
-      <c r="Q33" s="19"/>
-      <c r="R33" s="19"/>
-      <c r="S33" s="19"/>
+      <c r="K33" s="39"/>
+      <c r="L33" s="39"/>
+      <c r="M33" s="39"/>
+      <c r="N33" s="30"/>
+      <c r="O33" s="29"/>
+      <c r="P33" s="18"/>
+      <c r="Q33" s="18"/>
+      <c r="R33" s="18"/>
+      <c r="S33" s="18"/>
     </row>
     <row r="34" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="44"/>
-      <c r="B34" s="28"/>
-      <c r="C34" s="46"/>
-      <c r="D34" s="48"/>
-      <c r="E34" s="50"/>
-      <c r="F34" s="72"/>
-      <c r="G34" s="50"/>
-      <c r="H34" s="50"/>
-      <c r="I34" s="29"/>
-      <c r="J34" s="29"/>
-      <c r="K34" s="39"/>
-      <c r="L34" s="39"/>
-      <c r="M34" s="39"/>
-      <c r="N34" s="35"/>
-      <c r="O34" s="34"/>
-      <c r="P34" s="19"/>
-      <c r="Q34" s="19"/>
-      <c r="R34" s="19"/>
-      <c r="S34" s="19"/>
+      <c r="A34" s="45"/>
+      <c r="B34" s="25"/>
+      <c r="C34" s="47"/>
+      <c r="D34" s="49"/>
+      <c r="E34" s="34"/>
+      <c r="F34" s="34"/>
+      <c r="G34" s="51"/>
+      <c r="H34" s="34"/>
+      <c r="I34" s="34"/>
+      <c r="J34" s="37"/>
+      <c r="K34" s="40"/>
+      <c r="L34" s="40"/>
+      <c r="M34" s="40"/>
+      <c r="N34" s="31"/>
+      <c r="O34" s="29"/>
+      <c r="P34" s="18"/>
+      <c r="Q34" s="18"/>
+      <c r="R34" s="18"/>
+      <c r="S34" s="18"/>
     </row>
     <row r="35" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="41" t="s">
-        <v>29</v>
-      </c>
-      <c r="B35" s="25"/>
-      <c r="C35" s="45"/>
-      <c r="D35" s="47"/>
-      <c r="E35" s="49"/>
-      <c r="F35" s="71"/>
-      <c r="G35" s="49"/>
-      <c r="H35" s="49"/>
-      <c r="I35" s="26" t="str">
+      <c r="A35" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="B35" s="24"/>
+      <c r="C35" s="46"/>
+      <c r="D35" s="48"/>
+      <c r="E35" s="33"/>
+      <c r="F35" s="33"/>
+      <c r="G35" s="50"/>
+      <c r="H35" s="33"/>
+      <c r="I35" s="33" t="str">
         <f>IF(I36="","",(108468000*POWER(10,-0.4*I36))/0.171918)</f>
         <v/>
       </c>
-      <c r="J35" s="27" t="str">
+      <c r="J35" s="36" t="str">
         <f>IF(J36="","",0.00254*(POWER(10,(-0.4*J36))))</f>
         <v/>
       </c>
-      <c r="K35" s="38"/>
-      <c r="L35" s="38"/>
-      <c r="M35" s="38"/>
-      <c r="N35" s="37"/>
-      <c r="O35" s="34"/>
-      <c r="P35" s="19"/>
-      <c r="Q35" s="19"/>
-      <c r="R35" s="19"/>
-      <c r="S35" s="19"/>
+      <c r="K35" s="39"/>
+      <c r="L35" s="39"/>
+      <c r="M35" s="39"/>
+      <c r="N35" s="30"/>
+      <c r="O35" s="29"/>
+      <c r="P35" s="18"/>
+      <c r="Q35" s="18"/>
+      <c r="R35" s="18"/>
+      <c r="S35" s="18"/>
     </row>
     <row r="36" spans="1:19" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="42"/>
-      <c r="B36" s="30"/>
-      <c r="C36" s="100"/>
-      <c r="D36" s="101"/>
-      <c r="E36" s="102"/>
-      <c r="F36" s="103"/>
-      <c r="G36" s="102"/>
-      <c r="H36" s="102"/>
-      <c r="I36" s="31"/>
-      <c r="J36" s="31"/>
-      <c r="K36" s="40"/>
-      <c r="L36" s="40"/>
-      <c r="M36" s="40"/>
-      <c r="N36" s="36"/>
-      <c r="O36" s="34"/>
-      <c r="P36" s="19"/>
-      <c r="Q36" s="19"/>
-      <c r="R36" s="19"/>
-      <c r="S36" s="19"/>
+      <c r="A36" s="43"/>
+      <c r="B36" s="26"/>
+      <c r="C36" s="99"/>
+      <c r="D36" s="100"/>
+      <c r="E36" s="35"/>
+      <c r="F36" s="35"/>
+      <c r="G36" s="101"/>
+      <c r="H36" s="35"/>
+      <c r="I36" s="35"/>
+      <c r="J36" s="38"/>
+      <c r="K36" s="41"/>
+      <c r="L36" s="41"/>
+      <c r="M36" s="41"/>
+      <c r="N36" s="32"/>
+      <c r="O36" s="29"/>
+      <c r="P36" s="18"/>
+      <c r="Q36" s="18"/>
+      <c r="R36" s="18"/>
+      <c r="S36" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="127">
+  <mergeCells count="151">
     <mergeCell ref="C33:C34"/>
     <mergeCell ref="D33:D34"/>
     <mergeCell ref="E33:E34"/>
@@ -2671,6 +2514,7 @@
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="C15:N15"/>
     <mergeCell ref="C16:N16"/>
+    <mergeCell ref="N21:N22"/>
     <mergeCell ref="K25:K26"/>
     <mergeCell ref="L25:L26"/>
     <mergeCell ref="M25:M26"/>
@@ -2695,7 +2539,6 @@
     <mergeCell ref="D27:D28"/>
     <mergeCell ref="E27:E28"/>
     <mergeCell ref="G27:G28"/>
-    <mergeCell ref="K29:K30"/>
     <mergeCell ref="L29:L30"/>
     <mergeCell ref="M29:M30"/>
     <mergeCell ref="K27:K28"/>
@@ -2710,6 +2553,30 @@
     <mergeCell ref="K31:K32"/>
     <mergeCell ref="L31:L32"/>
     <mergeCell ref="M31:M32"/>
+    <mergeCell ref="N23:N24"/>
+    <mergeCell ref="N25:N26"/>
+    <mergeCell ref="N27:N28"/>
+    <mergeCell ref="N29:N30"/>
+    <mergeCell ref="N31:N32"/>
+    <mergeCell ref="N33:N34"/>
+    <mergeCell ref="N35:N36"/>
+    <mergeCell ref="I21:I22"/>
+    <mergeCell ref="I23:I24"/>
+    <mergeCell ref="I25:I26"/>
+    <mergeCell ref="I27:I28"/>
+    <mergeCell ref="I29:I30"/>
+    <mergeCell ref="I31:I32"/>
+    <mergeCell ref="I33:I34"/>
+    <mergeCell ref="I35:I36"/>
+    <mergeCell ref="J21:J22"/>
+    <mergeCell ref="J23:J24"/>
+    <mergeCell ref="J25:J26"/>
+    <mergeCell ref="J27:J28"/>
+    <mergeCell ref="J29:J30"/>
+    <mergeCell ref="J31:J32"/>
+    <mergeCell ref="J33:J34"/>
+    <mergeCell ref="J35:J36"/>
+    <mergeCell ref="K29:K30"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.3" right="0.25" top="0.3" bottom="0.1" header="0.3" footer="0.3"/>

</xml_diff>